<commit_message>
Transportation calibration edits (AVL, BHNVFEAL,BNVFE,TTS)
</commit_message>
<xml_diff>
--- a/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
+++ b/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murielle.gagnebin\Documents\02_ProjetsPays\01_DE\2004_EPS_Europe\eps-us-2.1.0\InputData\trans\AVL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-eu\InputData\trans\AVL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D1F81A-F13F-4571-A80A-362D09121777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577A112A-6853-4BFF-89CA-2BD20CDC9A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -18,12 +18,15 @@
     <sheet name="Data" sheetId="13" r:id="rId3"/>
     <sheet name="AVL" sheetId="10" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="100">
   <si>
     <t>ships</t>
   </si>
@@ -73,9 +76,6 @@
   </si>
   <si>
     <t>https://www.acea.be/uploads/publications/ACEA_Report_Vehicles_in_use-Europe_2019.pdf</t>
-  </si>
-  <si>
-    <t>LDVs &amp; HDVs Lifetimes</t>
   </si>
   <si>
     <t>ACEA (European Automobile Manufacturers Association)</t>
@@ -337,19 +337,43 @@
   <si>
     <t>Table 2.1: https://unctad.org/en/PublicationChapters/rmt2017ch2_en.pdf). We took the average age of world vessel fleets for freight, the average of the 3</t>
   </si>
+  <si>
+    <t>US AVLo settings (see US EPS)</t>
+  </si>
+  <si>
+    <t>other vehicle types: see notes below</t>
+  </si>
+  <si>
+    <t>freight LDVs &amp; passenger HDVs Lifetimes</t>
+  </si>
+  <si>
+    <t>Calibration edits: Passenger LDV fuel economy declines too quickly compared to Potencia if we use the ACEA value cited above. This</t>
+  </si>
+  <si>
+    <t>is due to the fact that the average lifetime does not capture the fact that many vehicles stay in circulation for much longer. We found a lifetime of 25</t>
+  </si>
+  <si>
+    <t>years best matches fleet fuel economy / stock turnover in the Potencia data set.</t>
+  </si>
+  <si>
+    <t>For freight HDVs, we also found fuel economy declines too quickly compared to Potencia if we use ACEA average lifetimes. We therefore use the average lifetime</t>
+  </si>
+  <si>
+    <t>of freight HDVs from the US EPS model, which are considerably longer than the ACEA lifetimes.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="7">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="###0.00_)"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="#,##0_)"/>
-    <numFmt numFmtId="174" formatCode="0.0%"/>
-    <numFmt numFmtId="175" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="###0.00_)"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0_)"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="33" x14ac:knownFonts="1">
     <font>
@@ -1044,7 +1068,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8">
@@ -1101,10 +1125,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="28" fillId="0" borderId="8">
+    <xf numFmtId="167" fontId="28" fillId="0" borderId="8">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1146,7 +1170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1156,89 +1180,89 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="36" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="62" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="62" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="63">
-    <cellStyle name="20 % - Akzent1" xfId="35" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="39" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="43" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="47" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="51" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="55" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="36" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="40" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="44" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="48" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="52" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="56" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="37" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="41" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="45" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="49" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="53" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="57" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="34" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="38" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="42" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="46" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="50" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="54" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="26" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="27" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="35" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="39" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="43" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="47" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="51" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="55" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="36" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="40" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="44" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="48" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="52" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="56" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="37" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="41" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="45" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="49" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="53" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="57" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="34" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="38" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="42" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="46" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="50" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="54" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Body: normal cell" xfId="3" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Data" xfId="14" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Data no deci" xfId="61" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Eingabe" xfId="25" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="33" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="32" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="9" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Footnotes: all except top row" xfId="12" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Gut" xfId="22" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Header: bottom row" xfId="2" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Header: top rows" xfId="4" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Hed Side" xfId="15" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Hed Side Regular" xfId="60" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Hed Top" xfId="59" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Hyperlink 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Komma" xfId="62" builtinId="3"/>
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Calculation" xfId="27" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="29" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="62" builtinId="3"/>
+    <cellStyle name="Data" xfId="14" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Data no deci" xfId="61" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Explanatory Text" xfId="32" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="9" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Footnotes: all except top row" xfId="12" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Good" xfId="22" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Header: bottom row" xfId="2" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Header: top rows" xfId="4" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="19" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="20" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="21" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hed Side" xfId="15" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Hed Side Regular" xfId="60" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Hed Top" xfId="59" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Input" xfId="25" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="28" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="24" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="31" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Prozent" xfId="16" builtinId="5"/>
-    <cellStyle name="Schlecht" xfId="23" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Section Break" xfId="8" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Section Break: parent row" xfId="5" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Table title" xfId="13" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Title-2" xfId="58" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Überschrift" xfId="17" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="18" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="19" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="20" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="21" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="28" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="30" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="29" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="31" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="26" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Percent" xfId="16" builtinId="5"/>
+    <cellStyle name="Section Break" xfId="8" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Section Break: parent row" xfId="5" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Table title" xfId="13" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Title" xfId="17" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Title-2" xfId="58" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Total" xfId="33" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="30" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1421,8 +1445,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7543801" y="466725"/>
-          <a:ext cx="5448300" cy="6598232"/>
+          <a:off x="7372351" y="444500"/>
+          <a:ext cx="5295900" cy="6268032"/>
           <a:chOff x="7534276" y="0"/>
           <a:chExt cx="5448300" cy="6598232"/>
         </a:xfrm>
@@ -2239,7 +2263,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2559,215 +2583,248 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="132.28515625" customWidth="1"/>
+    <col min="2" max="2" width="132.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="5">
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" s="5">
         <v>2019</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B18" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="9">
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="2:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B20" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B21" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B24" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B25" s="9">
         <v>2018</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B26" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B28" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B31" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B32" s="9">
         <v>2014</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B33" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B34" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B35" s="8"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="36" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="8"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>45</v>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{25C264B1-AF1E-490B-85D7-36E77BC789F2}"/>
-    <hyperlink ref="B27" r:id="rId2" xr:uid="{F3C9D0B8-A0BE-4BCC-8A76-AFE8441668D1}"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B27" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -2775,32 +2832,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E213073A-4DEC-4E38-B6FA-D48E27869689}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W45"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="42"/>
       <c r="R1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="R2" t="s">
+    <row r="45" spans="22:23" x14ac:dyDescent="0.35">
+      <c r="V45" s="6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="45" spans="22:23" x14ac:dyDescent="0.25">
-      <c r="V45" s="6" t="s">
+      <c r="W45" t="s">
         <v>86</v>
-      </c>
-      <c r="W45" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2810,57 +2867,57 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7449485A-9BBA-4FE7-AF5D-D63EA7CC6834}">
-  <dimension ref="A1:I57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.08984375" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="18"/>
       <c r="G2" s="25"/>
       <c r="H2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>44</v>
       </c>
       <c r="G3" s="36"/>
       <c r="H3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="21">
         <v>10.8</v>
@@ -2870,12 +2927,12 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="21">
         <v>10.9</v>
@@ -2885,12 +2942,12 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="21">
         <v>12.4</v>
@@ -2900,12 +2957,12 @@
         <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="21">
         <v>11.4</v>
@@ -2915,10 +2972,10 @@
         <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
@@ -2927,27 +2984,27 @@
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
     </row>
-    <row r="10" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="45.5" x14ac:dyDescent="0.35">
       <c r="A11" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>42</v>
-      </c>
       <c r="D11" s="30"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="25">
         <v>20.8</v>
@@ -2957,9 +3014,9 @@
       </c>
       <c r="D12" s="31"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="21">
         <v>16.201000000000001</v>
@@ -2969,9 +3026,9 @@
       </c>
       <c r="D13" s="32"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="21">
         <v>12.013999999999999</v>
@@ -2981,9 +3038,9 @@
       </c>
       <c r="D14" s="32"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="21">
         <v>11.443</v>
@@ -2993,9 +3050,9 @@
       </c>
       <c r="D15" s="32"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="21">
         <v>7.915</v>
@@ -3005,9 +3062,9 @@
       </c>
       <c r="D16" s="32"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="27">
         <v>10.823</v>
@@ -3018,9 +3075,9 @@
       </c>
       <c r="D17" s="31"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="26">
         <f>C17-C12</f>
@@ -3028,40 +3085,40 @@
       </c>
       <c r="D18" s="33"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="34">
         <f>ROUND(B12,0)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="34">
         <f>ROUND(SUMPRODUCT(B13:B16,C13:C16)/C18,0)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>1</v>
       </c>
@@ -3070,38 +3127,38 @@
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="C29" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" s="19">
         <v>30</v>
       </c>
       <c r="C30" s="19"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" s="19">
         <v>15</v>
       </c>
       <c r="C31" s="19"/>
     </row>
-    <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32" s="40">
         <v>11.4</v>
@@ -3110,9 +3167,9 @@
         <v>22800</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B33" s="40">
         <v>20</v>
@@ -3121,9 +3178,9 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34" s="40">
         <v>25</v>
@@ -3132,9 +3189,9 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" s="40">
         <v>20</v>
@@ -3143,9 +3200,9 @@
         <v>3401</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="40">
         <v>30</v>
@@ -3156,9 +3213,9 @@
       <c r="F36" s="37"/>
       <c r="G36" s="37"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" s="40">
         <v>34</v>
@@ -3169,9 +3226,9 @@
       <c r="G37" s="23"/>
       <c r="I37" s="38"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B38" s="40">
         <v>21</v>
@@ -3183,9 +3240,9 @@
       <c r="H38" s="38"/>
       <c r="I38" s="39"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B39" s="40">
         <v>17</v>
@@ -3196,9 +3253,9 @@
       <c r="F39" s="37"/>
       <c r="G39" s="23"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B40" s="40">
         <v>22</v>
@@ -3208,9 +3265,9 @@
       </c>
       <c r="G40" s="29"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B41" s="40">
         <v>24</v>
@@ -3220,9 +3277,9 @@
       </c>
       <c r="F41" s="29"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B42" s="40">
         <v>12</v>
@@ -3232,9 +3289,9 @@
       </c>
       <c r="F42" s="29"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B43" s="40">
         <v>30</v>
@@ -3244,9 +3301,9 @@
       </c>
       <c r="F43" s="29"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" s="34">
         <f>ROUND(SUMPRODUCT(B32:B43,C32:C43)/C44,0)</f>
@@ -3257,12 +3314,12 @@
         <v>57516</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>0</v>
       </c>
@@ -3271,15 +3328,15 @@
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="19" t="s">
         <v>11</v>
       </c>
@@ -3287,7 +3344,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="19" t="s">
         <v>10</v>
       </c>
@@ -3295,7 +3352,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>7</v>
       </c>
@@ -3303,20 +3360,20 @@
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="19" t="s">
         <v>75</v>
-      </c>
-      <c r="B56" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="19" t="s">
-        <v>76</v>
       </c>
       <c r="B57" s="25">
         <v>9.0500000000000007</v>
@@ -3326,8 +3383,93 @@
         <v>9</v>
       </c>
     </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61">
+        <v>13</v>
+      </c>
+      <c r="C61">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62">
+        <v>23</v>
+      </c>
+      <c r="C62">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63">
+        <v>24</v>
+      </c>
+      <c r="C63">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>34</v>
+      </c>
+      <c r="C64">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65">
+        <v>33</v>
+      </c>
+      <c r="C65">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66">
+        <v>17</v>
+      </c>
+      <c r="C66">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3339,17 +3481,17 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.6328125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>12</v>
       </c>
@@ -3360,20 +3502,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="15">
-        <f>Data!C4</f>
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C2" s="15">
         <f>Data!C5</f>
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -3382,11 +3523,11 @@
         <v>11</v>
       </c>
       <c r="C3" s="15">
-        <f>Data!C6</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <f>Data!C62</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3399,7 +3540,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -3412,7 +3553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -3425,7 +3566,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Re-calibrated transport sector using BAADTbVT rather than cargo distance
</commit_message>
<xml_diff>
--- a/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
+++ b/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\trans\AVL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FCD5EF-BAFF-4FF2-BC04-1FC171B6B093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BE6B5C2-6CE0-4290-841C-DE5561F66419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="61905" yWindow="3135" windowWidth="22140" windowHeight="13245" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -24,6 +24,9 @@
     <sheet name="SoCDTtiNTY-frgt" sheetId="20" r:id="rId9"/>
     <sheet name="AVL" sheetId="10" r:id="rId10"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId11"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3744,15 +3747,6 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="58" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3763,6 +3757,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3871,6 +3874,58 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="About"/>
+      <sheetName val="ACEA Stock"/>
+      <sheetName val="ACEA Sales"/>
+      <sheetName val="calcs"/>
+      <sheetName val="SoCDTtiNTY-psgr"/>
+      <sheetName val="SoCDTtiNTY-frgt"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="4">
+          <cell r="C4">
+            <v>5.3489407911602317E-2</v>
+          </cell>
+          <cell r="D4">
+            <v>4.0324092592718512E-2</v>
+          </cell>
+          <cell r="E4">
+            <v>3.8857139556321266E-2</v>
+          </cell>
+          <cell r="F4">
+            <v>3.6725304130200163E-2</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="D5">
+            <v>4.2633856773290693E-2</v>
+          </cell>
+          <cell r="E5">
+            <v>4.359738562091503E-2</v>
+          </cell>
+          <cell r="F5">
+            <v>4.0383085705738106E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4435,7 +4490,7 @@
       </c>
       <c r="B2" s="70">
         <f>ROUND(1/'SoCDTtiNTY-psgr'!B2,0)</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="70">
         <f>ROUND(1/'SoCDTtiNTY-frgt'!B2,0)</f>
@@ -39427,62 +39482,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
-      <c r="T1" s="80"/>
-      <c r="U1" s="80"/>
-      <c r="V1" s="80"/>
-      <c r="W1" s="80"/>
-      <c r="X1" s="80"/>
-      <c r="Y1" s="80"/>
-      <c r="Z1" s="80"/>
-      <c r="AA1" s="80"/>
-      <c r="AB1" s="80"/>
-      <c r="AC1" s="81"/>
-      <c r="AD1" s="81"/>
-      <c r="AE1" s="81"/>
-      <c r="AF1" s="81"/>
-      <c r="AG1" s="81"/>
-      <c r="AH1" s="81"/>
-      <c r="AI1" s="81"/>
-      <c r="AJ1" s="81"/>
-      <c r="AK1" s="81"/>
-      <c r="AL1" s="81"/>
-      <c r="AM1" s="81"/>
-      <c r="AN1" s="81"/>
-      <c r="AO1" s="81"/>
-      <c r="AP1" s="81"/>
-      <c r="AQ1" s="81"/>
-      <c r="AR1" s="81"/>
-      <c r="AS1" s="81"/>
-      <c r="AT1" s="81"/>
-      <c r="AU1" s="81"/>
-      <c r="AV1" s="81"/>
-      <c r="AW1" s="81"/>
-      <c r="AX1" s="81"/>
-      <c r="AY1" s="81"/>
-      <c r="AZ1" s="81"/>
-      <c r="BA1" s="81"/>
-      <c r="BB1" s="81"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
+      <c r="AG1" s="78"/>
+      <c r="AH1" s="78"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="78"/>
+      <c r="AK1" s="78"/>
+      <c r="AL1" s="78"/>
+      <c r="AM1" s="78"/>
+      <c r="AN1" s="78"/>
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="78"/>
+      <c r="AQ1" s="78"/>
+      <c r="AR1" s="78"/>
+      <c r="AS1" s="78"/>
+      <c r="AT1" s="78"/>
+      <c r="AU1" s="78"/>
+      <c r="AV1" s="78"/>
+      <c r="AW1" s="78"/>
+      <c r="AX1" s="78"/>
+      <c r="AY1" s="78"/>
+      <c r="AZ1" s="78"/>
+      <c r="BA1" s="78"/>
+      <c r="BB1" s="78"/>
     </row>
     <row r="2" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="38"/>
@@ -41505,65 +41560,65 @@
       <c r="BB20" s="59"/>
     </row>
     <row r="21" spans="1:54" s="63" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="82" t="s">
+      <c r="A21" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="82"/>
-      <c r="C21" s="82"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="82"/>
-      <c r="F21" s="82"/>
-      <c r="G21" s="82"/>
-      <c r="H21" s="82"/>
-      <c r="I21" s="82"/>
-      <c r="J21" s="82"/>
-      <c r="K21" s="82"/>
-      <c r="L21" s="82"/>
-      <c r="M21" s="82"/>
-      <c r="N21" s="82"/>
-      <c r="O21" s="82"/>
-      <c r="P21" s="82"/>
-      <c r="Q21" s="82"/>
+      <c r="B21" s="79"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="79"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="79"/>
+      <c r="M21" s="79"/>
+      <c r="N21" s="79"/>
+      <c r="O21" s="79"/>
+      <c r="P21" s="79"/>
+      <c r="Q21" s="79"/>
     </row>
     <row r="22" spans="1:54" s="63" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="83"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="83"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="83"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="83"/>
-      <c r="J22" s="83"/>
-      <c r="K22" s="83"/>
-      <c r="L22" s="83"/>
-      <c r="M22" s="83"/>
-      <c r="N22" s="83"/>
-      <c r="O22" s="83"/>
-      <c r="P22" s="83"/>
-      <c r="Q22" s="83"/>
+      <c r="A22" s="80"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="80"/>
+      <c r="M22" s="80"/>
+      <c r="N22" s="80"/>
+      <c r="O22" s="80"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="80"/>
     </row>
     <row r="23" spans="1:54" s="63" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="83" t="s">
+      <c r="A23" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="83"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="83"/>
-      <c r="J23" s="83"/>
-      <c r="K23" s="83"/>
-      <c r="L23" s="83"/>
-      <c r="M23" s="83"/>
-      <c r="N23" s="83"/>
-      <c r="O23" s="83"/>
-      <c r="P23" s="83"/>
-      <c r="Q23" s="83"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="80"/>
+      <c r="L23" s="80"/>
+      <c r="M23" s="80"/>
+      <c r="N23" s="80"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="80"/>
+      <c r="Q23" s="80"/>
     </row>
     <row r="24" spans="1:54" s="63" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="76" t="s">
@@ -41608,86 +41663,86 @@
       <c r="Q25" s="76"/>
     </row>
     <row r="26" spans="1:54" s="63" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="77" t="s">
+      <c r="A26" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="77"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="77"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="77"/>
-      <c r="K26" s="77"/>
-      <c r="L26" s="77"/>
-      <c r="M26" s="77"/>
-      <c r="N26" s="77"/>
-      <c r="O26" s="77"/>
-      <c r="P26" s="77"/>
-      <c r="Q26" s="77"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="81"/>
+      <c r="G26" s="81"/>
+      <c r="H26" s="81"/>
+      <c r="I26" s="81"/>
+      <c r="J26" s="81"/>
+      <c r="K26" s="81"/>
+      <c r="L26" s="81"/>
+      <c r="M26" s="81"/>
+      <c r="N26" s="81"/>
+      <c r="O26" s="81"/>
+      <c r="P26" s="81"/>
+      <c r="Q26" s="81"/>
     </row>
     <row r="27" spans="1:54" s="63" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="77"/>
-      <c r="B27" s="77"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="77"/>
-      <c r="E27" s="77"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="77"/>
-      <c r="J27" s="77"/>
-      <c r="K27" s="77"/>
-      <c r="L27" s="77"/>
-      <c r="M27" s="77"/>
-      <c r="N27" s="77"/>
-      <c r="O27" s="77"/>
-      <c r="P27" s="77"/>
-      <c r="Q27" s="77"/>
+      <c r="A27" s="81"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="81"/>
+      <c r="I27" s="81"/>
+      <c r="J27" s="81"/>
+      <c r="K27" s="81"/>
+      <c r="L27" s="81"/>
+      <c r="M27" s="81"/>
+      <c r="N27" s="81"/>
+      <c r="O27" s="81"/>
+      <c r="P27" s="81"/>
+      <c r="Q27" s="81"/>
     </row>
     <row r="28" spans="1:54" s="63" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="78" t="s">
+      <c r="A28" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="B28" s="78"/>
-      <c r="C28" s="78"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="78"/>
-      <c r="I28" s="78"/>
-      <c r="J28" s="78"/>
-      <c r="K28" s="78"/>
-      <c r="L28" s="78"/>
-      <c r="M28" s="78"/>
-      <c r="N28" s="78"/>
-      <c r="O28" s="78"/>
-      <c r="P28" s="78"/>
-      <c r="Q28" s="78"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="82"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="82"/>
+      <c r="N28" s="82"/>
+      <c r="O28" s="82"/>
+      <c r="P28" s="82"/>
+      <c r="Q28" s="82"/>
     </row>
     <row r="29" spans="1:54" s="63" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="79" t="s">
+      <c r="A29" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="79"/>
-      <c r="C29" s="79"/>
-      <c r="D29" s="79"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="79"/>
-      <c r="G29" s="79"/>
-      <c r="H29" s="79"/>
-      <c r="I29" s="79"/>
-      <c r="J29" s="79"/>
-      <c r="K29" s="79"/>
-      <c r="L29" s="79"/>
-      <c r="M29" s="79"/>
-      <c r="N29" s="79"/>
-      <c r="O29" s="79"/>
-      <c r="P29" s="79"/>
-      <c r="Q29" s="79"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="83"/>
+      <c r="D29" s="83"/>
+      <c r="E29" s="83"/>
+      <c r="F29" s="83"/>
+      <c r="G29" s="83"/>
+      <c r="H29" s="83"/>
+      <c r="I29" s="83"/>
+      <c r="J29" s="83"/>
+      <c r="K29" s="83"/>
+      <c r="L29" s="83"/>
+      <c r="M29" s="83"/>
+      <c r="N29" s="83"/>
+      <c r="O29" s="83"/>
+      <c r="P29" s="83"/>
+      <c r="Q29" s="83"/>
     </row>
     <row r="33" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="34" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -41720,17 +41775,17 @@
     <row r="61" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A25:Q25"/>
+    <mergeCell ref="A26:Q26"/>
+    <mergeCell ref="A27:Q27"/>
+    <mergeCell ref="A28:Q28"/>
+    <mergeCell ref="A29:Q29"/>
     <mergeCell ref="A24:Q24"/>
     <mergeCell ref="A1:AB1"/>
     <mergeCell ref="AC1:BB1"/>
     <mergeCell ref="A21:Q21"/>
     <mergeCell ref="A22:Q22"/>
     <mergeCell ref="A23:Q23"/>
-    <mergeCell ref="A25:Q25"/>
-    <mergeCell ref="A26:Q26"/>
-    <mergeCell ref="A27:Q27"/>
-    <mergeCell ref="A28:Q28"/>
-    <mergeCell ref="A29:Q29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -42344,25 +42399,32 @@
         <v>48</v>
       </c>
       <c r="B2">
-        <v>3.8635512093079978E-2</v>
+        <f>AVERAGE([1]calcs!$C4:$F4)</f>
+        <v>4.234898604771057E-2</v>
       </c>
       <c r="C2">
-        <v>3.8635512093079978E-2</v>
+        <f>AVERAGE([1]calcs!$C4:$F4)</f>
+        <v>4.234898604771057E-2</v>
       </c>
       <c r="D2">
-        <v>3.8635512093079978E-2</v>
+        <f>AVERAGE([1]calcs!$C4:$F4)</f>
+        <v>4.234898604771057E-2</v>
       </c>
       <c r="E2">
-        <v>3.8635512093079978E-2</v>
+        <f>AVERAGE([1]calcs!$C4:$F4)</f>
+        <v>4.234898604771057E-2</v>
       </c>
       <c r="F2">
-        <v>3.8635512093079978E-2</v>
+        <f>AVERAGE([1]calcs!$C4:$F4)</f>
+        <v>4.234898604771057E-2</v>
       </c>
       <c r="G2">
-        <v>3.8635512093079978E-2</v>
+        <f>AVERAGE([1]calcs!$C4:$F4)</f>
+        <v>4.234898604771057E-2</v>
       </c>
       <c r="H2">
-        <v>3.8635512093079978E-2</v>
+        <f>AVERAGE([1]calcs!$C4:$F4)</f>
+        <v>4.234898604771057E-2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -42370,24 +42432,31 @@
         <v>51</v>
       </c>
       <c r="B3">
+        <f>AVERAGE([1]calcs!$D5:$F5)</f>
         <v>4.2204776033314607E-2</v>
       </c>
       <c r="C3">
+        <f>AVERAGE([1]calcs!$D5:$F5)</f>
         <v>4.2204776033314607E-2</v>
       </c>
       <c r="D3">
+        <f>AVERAGE([1]calcs!$D5:$F5)</f>
         <v>4.2204776033314607E-2</v>
       </c>
       <c r="E3">
+        <f>AVERAGE([1]calcs!$D5:$F5)</f>
         <v>4.2204776033314607E-2</v>
       </c>
       <c r="F3">
+        <f>AVERAGE([1]calcs!$D5:$F5)</f>
         <v>4.2204776033314607E-2</v>
       </c>
       <c r="G3">
+        <f>AVERAGE([1]calcs!$D5:$F5)</f>
         <v>4.2204776033314607E-2</v>
       </c>
       <c r="H3">
+        <f>AVERAGE([1]calcs!$D5:$F5)</f>
         <v>4.2204776033314607E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Calibrates frgt-LDV 2022/23 historical sales and future projections
</commit_message>
<xml_diff>
--- a/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
+++ b/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\trans\AVL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BE6B5C2-6CE0-4290-841C-DE5561F66419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC4B8C5-5EAF-48BE-B90A-2D373A887F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61905" yWindow="3135" windowWidth="22140" windowHeight="13245" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58740" yWindow="1140" windowWidth="22140" windowHeight="13230" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -24,9 +24,6 @@
     <sheet name="SoCDTtiNTY-frgt" sheetId="20" r:id="rId9"/>
     <sheet name="AVL" sheetId="10" r:id="rId10"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId11"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3876,58 +3873,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="About"/>
-      <sheetName val="ACEA Stock"/>
-      <sheetName val="ACEA Sales"/>
-      <sheetName val="calcs"/>
-      <sheetName val="SoCDTtiNTY-psgr"/>
-      <sheetName val="SoCDTtiNTY-frgt"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="4">
-          <cell r="C4">
-            <v>5.3489407911602317E-2</v>
-          </cell>
-          <cell r="D4">
-            <v>4.0324092592718512E-2</v>
-          </cell>
-          <cell r="E4">
-            <v>3.8857139556321266E-2</v>
-          </cell>
-          <cell r="F4">
-            <v>3.6725304130200163E-2</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>4.2633856773290693E-2</v>
-          </cell>
-          <cell r="E5">
-            <v>4.359738562091503E-2</v>
-          </cell>
-          <cell r="F5">
-            <v>4.0383085705738106E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -4494,7 +4439,7 @@
       </c>
       <c r="C2" s="70">
         <f>ROUND(1/'SoCDTtiNTY-frgt'!B2,0)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -42359,7 +42304,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -42399,32 +42344,25 @@
         <v>48</v>
       </c>
       <c r="B2">
-        <f>AVERAGE([1]calcs!$C4:$F4)</f>
-        <v>4.234898604771057E-2</v>
+        <v>4.2348985999999998E-2</v>
       </c>
       <c r="C2">
-        <f>AVERAGE([1]calcs!$C4:$F4)</f>
-        <v>4.234898604771057E-2</v>
+        <v>4.2348985999999998E-2</v>
       </c>
       <c r="D2">
-        <f>AVERAGE([1]calcs!$C4:$F4)</f>
-        <v>4.234898604771057E-2</v>
+        <v>4.2348985999999998E-2</v>
       </c>
       <c r="E2">
-        <f>AVERAGE([1]calcs!$C4:$F4)</f>
-        <v>4.234898604771057E-2</v>
+        <v>4.2348985999999998E-2</v>
       </c>
       <c r="F2">
-        <f>AVERAGE([1]calcs!$C4:$F4)</f>
-        <v>4.234898604771057E-2</v>
+        <v>4.2348985999999998E-2</v>
       </c>
       <c r="G2">
-        <f>AVERAGE([1]calcs!$C4:$F4)</f>
-        <v>4.234898604771057E-2</v>
+        <v>4.2348985999999998E-2</v>
       </c>
       <c r="H2">
-        <f>AVERAGE([1]calcs!$C4:$F4)</f>
-        <v>4.234898604771057E-2</v>
+        <v>4.2348985999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -42432,32 +42370,25 @@
         <v>51</v>
       </c>
       <c r="B3">
-        <f>AVERAGE([1]calcs!$D5:$F5)</f>
-        <v>4.2204776033314607E-2</v>
+        <v>4.2204775999999999E-2</v>
       </c>
       <c r="C3">
-        <f>AVERAGE([1]calcs!$D5:$F5)</f>
-        <v>4.2204776033314607E-2</v>
+        <v>4.2204775999999999E-2</v>
       </c>
       <c r="D3">
-        <f>AVERAGE([1]calcs!$D5:$F5)</f>
-        <v>4.2204776033314607E-2</v>
+        <v>4.2204775999999999E-2</v>
       </c>
       <c r="E3">
-        <f>AVERAGE([1]calcs!$D5:$F5)</f>
-        <v>4.2204776033314607E-2</v>
+        <v>4.2204775999999999E-2</v>
       </c>
       <c r="F3">
-        <f>AVERAGE([1]calcs!$D5:$F5)</f>
-        <v>4.2204776033314607E-2</v>
+        <v>4.2204775999999999E-2</v>
       </c>
       <c r="G3">
-        <f>AVERAGE([1]calcs!$D5:$F5)</f>
-        <v>4.2204776033314607E-2</v>
+        <v>4.2204775999999999E-2</v>
       </c>
       <c r="H3">
-        <f>AVERAGE([1]calcs!$D5:$F5)</f>
-        <v>4.2204776033314607E-2</v>
+        <v>4.2204775999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -42577,7 +42508,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H8"/>
+      <selection sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -42586,29 +42517,29 @@
     <col min="2" max="8" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="30" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>853</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" t="s">
         <v>854</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" t="s">
         <v>855</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" t="s">
         <v>856</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" t="s">
         <v>857</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" t="s">
         <v>858</v>
       </c>
-      <c r="G1" s="72" t="s">
+      <c r="G1" t="s">
         <v>859</v>
       </c>
-      <c r="H1" s="72" t="s">
+      <c r="H1" t="s">
         <v>860</v>
       </c>
     </row>
@@ -42617,25 +42548,25 @@
         <v>48</v>
       </c>
       <c r="B2">
-        <v>5.190582462648987E-2</v>
+        <v>5.5380247000000001E-2</v>
       </c>
       <c r="C2">
-        <v>5.190582462648987E-2</v>
+        <v>5.5380247000000001E-2</v>
       </c>
       <c r="D2">
-        <v>5.190582462648987E-2</v>
+        <v>5.5380247000000001E-2</v>
       </c>
       <c r="E2">
-        <v>5.190582462648987E-2</v>
+        <v>5.5380247000000001E-2</v>
       </c>
       <c r="F2">
-        <v>5.190582462648987E-2</v>
+        <v>5.5380247000000001E-2</v>
       </c>
       <c r="G2">
-        <v>5.190582462648987E-2</v>
+        <v>5.5380247000000001E-2</v>
       </c>
       <c r="H2">
-        <v>5.190582462648987E-2</v>
+        <v>5.5380247000000001E-2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -42643,25 +42574,25 @@
         <v>51</v>
       </c>
       <c r="B3">
-        <v>5.0582439096787349E-2</v>
+        <v>5.0582439E-2</v>
       </c>
       <c r="C3">
-        <v>5.0582439096787349E-2</v>
+        <v>5.0582439E-2</v>
       </c>
       <c r="D3">
-        <v>5.0582439096787349E-2</v>
+        <v>5.0582439E-2</v>
       </c>
       <c r="E3">
-        <v>5.0582439096787349E-2</v>
+        <v>5.0582439E-2</v>
       </c>
       <c r="F3">
-        <v>5.0582439096787349E-2</v>
+        <v>5.0582439E-2</v>
       </c>
       <c r="G3">
-        <v>5.0582439096787349E-2</v>
+        <v>5.0582439E-2</v>
       </c>
       <c r="H3">
-        <v>5.0582439096787349E-2</v>
+        <v>5.0582439E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Calibrate frgt-HDV sales for 2022/23 and projected
</commit_message>
<xml_diff>
--- a/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
+++ b/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\trans\AVL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC4B8C5-5EAF-48BE-B90A-2D373A887F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5341A9CB-39DA-4C49-9AE4-C4318F736D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58740" yWindow="1140" windowWidth="22140" windowHeight="13230" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="61650" yWindow="3240" windowWidth="22140" windowHeight="13245" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -4408,7 +4408,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4452,7 +4452,7 @@
       </c>
       <c r="C3" s="70">
         <f>ROUND(1/'SoCDTtiNTY-frgt'!B3,0)</f>
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -42508,7 +42508,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H7"/>
+      <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -42574,25 +42574,25 @@
         <v>51</v>
       </c>
       <c r="B3">
-        <v>5.0582439E-2</v>
+        <v>6.0404717788497909E-2</v>
       </c>
       <c r="C3">
-        <v>5.0582439E-2</v>
+        <v>6.0404717788497909E-2</v>
       </c>
       <c r="D3">
-        <v>5.0582439E-2</v>
+        <v>6.0404717788497909E-2</v>
       </c>
       <c r="E3">
-        <v>5.0582439E-2</v>
+        <v>6.0404717788497909E-2</v>
       </c>
       <c r="F3">
-        <v>5.0582439E-2</v>
+        <v>6.0404717788497909E-2</v>
       </c>
       <c r="G3">
-        <v>5.0582439E-2</v>
+        <v>6.0404717788497909E-2</v>
       </c>
       <c r="H3">
-        <v>5.0582439E-2</v>
+        <v>6.0404717788497909E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Calibrates psgr-HDVs -- transportation calibration complete
</commit_message>
<xml_diff>
--- a/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
+++ b/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\trans\AVL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5341A9CB-39DA-4C49-9AE4-C4318F736D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9551FC-53A9-483A-91CF-10004F72B6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61650" yWindow="3240" windowWidth="22140" windowHeight="13245" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="570" windowWidth="22140" windowHeight="13245" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -4448,7 +4448,7 @@
       </c>
       <c r="B3" s="74">
         <f>ROUND(1/'SoCDTtiNTY-psgr'!B3,0)</f>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C3" s="70">
         <f>ROUND(1/'SoCDTtiNTY-frgt'!B3,0)</f>
@@ -42304,7 +42304,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B3" sqref="B3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -42370,25 +42370,25 @@
         <v>51</v>
       </c>
       <c r="B3">
-        <v>4.2204775999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C3">
-        <v>4.2204775999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="D3">
-        <v>4.2204775999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="E3">
-        <v>4.2204775999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F3">
-        <v>4.2204775999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="G3">
-        <v>4.2204775999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="H3">
-        <v>4.2204775999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>